<commit_message>
updated the files for release version in report 20140627
</commit_message>
<xml_diff>
--- a/引脚使用情况.xlsx
+++ b/引脚使用情况.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="PORT" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
   <si>
     <t>液晶使用</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -277,6 +277,70 @@
   <si>
     <t>N_code</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>CAP2.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更换使用CAP2.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P0.4 (AF3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAT0.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P1.29 (AF3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAT2.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P0.6 (AF3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更换使用MAT2.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>匹配输出触发ADC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>由于MAT2.0不能直接触发ADC，故将MAT2.0接到ADC触发引脚P210，由P210直接触发。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P210</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P2.10（输入IO）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>由MAT2.0接入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2014_06_11修改</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAT0.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P3.26 (AF3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -327,7 +391,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -370,6 +434,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -385,14 +455,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
@@ -410,10 +477,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -423,6 +486,22 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -598,11 +677,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="89574016"/>
-        <c:axId val="89579904"/>
+        <c:axId val="73685248"/>
+        <c:axId val="73707520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89574016"/>
+        <c:axId val="73685248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -626,12 +705,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89579904"/>
+        <c:crossAx val="73707520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89579904"/>
+        <c:axId val="73707520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -639,21 +718,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89574016"/>
+        <c:crossAx val="73685248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1161,8 +1239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1170,60 +1248,61 @@
     <col min="1" max="1" width="8.625" customWidth="1"/>
     <col min="9" max="9" width="12.5" customWidth="1"/>
     <col min="10" max="10" width="15.25" customWidth="1"/>
-    <col min="12" max="12" width="13.375" customWidth="1"/>
+    <col min="12" max="12" width="19.875" customWidth="1"/>
+    <col min="13" max="13" width="14.875" customWidth="1"/>
     <col min="15" max="15" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="16.5" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="E1" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="11"/>
+      <c r="H1" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="I1" s="11"/>
+      <c r="K1" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="L1" s="11"/>
+      <c r="N1" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="O1" s="2"/>
+      <c r="O1" s="11"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="2"/>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="E2" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>48</v>
       </c>
       <c r="H2" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>61</v>
       </c>
       <c r="J2" t="s">
         <v>66</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>63</v>
       </c>
       <c r="M2" t="s">
@@ -1232,230 +1311,297 @@
       <c r="N2" t="s">
         <v>58</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="2"/>
       <c r="C3" t="s">
         <v>18</v>
       </c>
       <c r="E3" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>49</v>
       </c>
       <c r="H3" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>62</v>
       </c>
       <c r="J3" t="s">
         <v>67</v>
       </c>
+      <c r="K3" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M3" t="s">
+        <v>73</v>
+      </c>
       <c r="N3" t="s">
         <v>59</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="2"/>
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="E4" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="2"/>
       <c r="C5" t="s">
         <v>20</v>
       </c>
       <c r="E5" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="2"/>
       <c r="C6" t="s">
         <v>21</v>
       </c>
+      <c r="K6" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="L6" s="11"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="2"/>
       <c r="C7" t="s">
         <v>22</v>
       </c>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="2"/>
       <c r="C8" t="s">
         <v>23</v>
       </c>
+      <c r="K8" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="L8" t="s">
+        <v>76</v>
+      </c>
+      <c r="M8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="2"/>
       <c r="C9" t="s">
         <v>24</v>
       </c>
+      <c r="K9" t="s">
+        <v>77</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M9" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="2"/>
       <c r="C10" t="s">
         <v>25</v>
       </c>
+      <c r="K10" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="2"/>
       <c r="C11" t="s">
         <v>26</v>
       </c>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="2"/>
       <c r="C12" t="s">
         <v>27</v>
       </c>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="2"/>
       <c r="C13" t="s">
         <v>28</v>
       </c>
+      <c r="K13" t="s">
+        <v>82</v>
+      </c>
+      <c r="L13" t="s">
+        <v>83</v>
+      </c>
+      <c r="M13" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="2"/>
       <c r="C14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="2"/>
       <c r="C15" t="s">
         <v>30</v>
       </c>
+      <c r="K15" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
+      <c r="B16" s="2"/>
       <c r="C16" t="s">
         <v>31</v>
       </c>
+      <c r="K16" t="s">
+        <v>86</v>
+      </c>
+      <c r="L16" s="16" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="3"/>
+      <c r="B17" s="2"/>
       <c r="C17" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="6"/>
+      <c r="B18" s="5"/>
       <c r="C18" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="6"/>
+      <c r="B19" s="5"/>
       <c r="C19" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="6"/>
+      <c r="B20" s="5"/>
       <c r="C20" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="6"/>
+      <c r="B21" s="5"/>
       <c r="C21" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="4"/>
+      <c r="B22" s="3"/>
       <c r="C22" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="K6:L7"/>
+    <mergeCell ref="K10:M12"/>
+    <mergeCell ref="K15:M15"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="N1:O1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1467,1113 +1613,1113 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="16384" width="9" style="10"/>
+    <col min="1" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>69</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="8" t="s">
         <v>69</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="9" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="11">
+      <c r="A3" s="8">
         <v>0.5</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="10">
         <f>10^(A3/20)</f>
         <v>1.0592537251772889</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="9">
         <f>2*A3+192</f>
         <v>193</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="8">
         <v>-0.5</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="10">
         <f>10^(D3/20)</f>
         <v>0.94406087628592339</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="9">
         <f>2*D3+192</f>
         <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="11">
+      <c r="A4" s="8">
         <v>1</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="10">
         <f t="shared" ref="B4:B65" si="0">10^(A4/20)</f>
         <v>1.1220184543019636</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="9">
         <f t="shared" ref="C4:C65" si="1">2*A4+192</f>
         <v>194</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="8">
         <v>-1</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="10">
         <f t="shared" ref="E4:E25" si="2">10^(D4/20)</f>
         <v>0.89125093813374545</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="9">
         <f t="shared" ref="F4:F25" si="3">2*D4+192</f>
         <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="11">
+      <c r="A5" s="8">
         <v>1.5</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="10">
         <f t="shared" si="0"/>
         <v>1.1885022274370185</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="9">
         <f t="shared" si="1"/>
         <v>195</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="8">
         <v>-1.5</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="10">
         <f t="shared" si="2"/>
         <v>0.84139514164519502</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="9">
         <f t="shared" si="3"/>
         <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="11">
+      <c r="A6" s="8">
         <v>2</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="10">
         <f t="shared" si="0"/>
         <v>1.2589254117941673</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="9">
         <f t="shared" si="1"/>
         <v>196</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="8">
         <v>-2</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="10">
         <f t="shared" si="2"/>
         <v>0.79432823472428149</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="9">
         <f t="shared" si="3"/>
         <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="11">
+      <c r="A7" s="8">
         <v>2.5</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="10">
         <f t="shared" si="0"/>
         <v>1.333521432163324</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="9">
         <f t="shared" si="1"/>
         <v>197</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="8">
         <v>-2.5</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="10">
         <f t="shared" si="2"/>
         <v>0.74989420933245587</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="9">
         <f t="shared" si="3"/>
         <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="11">
+      <c r="A8" s="8">
         <v>3</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="10">
         <f t="shared" si="0"/>
         <v>1.4125375446227544</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="9">
         <f t="shared" si="1"/>
         <v>198</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="8">
         <v>-3</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="10">
         <f t="shared" si="2"/>
         <v>0.70794578438413791</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="9">
         <f t="shared" si="3"/>
         <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="11">
+      <c r="A9" s="8">
         <v>3.5</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="10">
         <f t="shared" si="0"/>
         <v>1.4962356560944334</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="9">
         <f t="shared" si="1"/>
         <v>199</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="8">
         <v>-3.5</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="10">
         <f t="shared" si="2"/>
         <v>0.66834391756861455</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="9">
         <f t="shared" si="3"/>
         <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="11">
+      <c r="A10" s="8">
         <v>4</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="10">
         <f t="shared" si="0"/>
         <v>1.5848931924611136</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="9">
         <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="8">
         <v>-4</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="10">
         <f t="shared" si="2"/>
         <v>0.63095734448019325</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="9">
         <f t="shared" si="3"/>
         <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="11">
+      <c r="A11" s="8">
         <v>4.5</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="10">
         <f t="shared" si="0"/>
         <v>1.6788040181225605</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="9">
         <f t="shared" si="1"/>
         <v>201</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="8">
         <v>-4.5</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="10">
         <f t="shared" si="2"/>
         <v>0.59566214352901037</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="9">
         <f t="shared" si="3"/>
         <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="11">
+      <c r="A12" s="8">
         <v>5</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="10">
         <f t="shared" si="0"/>
         <v>1.778279410038923</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="9">
         <f t="shared" si="1"/>
         <v>202</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="8">
         <v>-5</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="10">
         <f t="shared" si="2"/>
         <v>0.56234132519034907</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="9">
         <f t="shared" si="3"/>
         <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="11">
+      <c r="A13" s="8">
         <v>5.5</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="10">
         <f t="shared" si="0"/>
         <v>1.8836490894898008</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="9">
         <f t="shared" si="1"/>
         <v>203</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="8">
         <v>-5.5</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="10">
         <f t="shared" si="2"/>
         <v>0.53088444423098824</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="9">
         <f t="shared" si="3"/>
         <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="11">
+      <c r="A14" s="8">
         <v>6</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="10">
         <f t="shared" si="0"/>
         <v>1.9952623149688797</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="9">
         <f t="shared" si="1"/>
         <v>204</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="8">
         <v>-6</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="10">
         <f t="shared" si="2"/>
         <v>0.50118723362727224</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="9">
         <f t="shared" si="3"/>
         <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="11">
+      <c r="A15" s="8">
         <v>6.5</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="10">
         <f t="shared" si="0"/>
         <v>2.1134890398366468</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="9">
         <f t="shared" si="1"/>
         <v>205</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="8">
         <v>-6.5</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="10">
         <f t="shared" si="2"/>
         <v>0.47315125896148047</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="9">
         <f t="shared" si="3"/>
         <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="11">
+      <c r="A16" s="8">
         <v>7</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="10">
         <f t="shared" si="0"/>
         <v>2.2387211385683394</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="9">
         <f t="shared" si="1"/>
         <v>206</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="8">
         <v>-7</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="10">
         <f t="shared" si="2"/>
         <v>0.44668359215096315</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="9">
         <f t="shared" si="3"/>
         <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="11">
+      <c r="A17" s="8">
         <v>7.5</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="10">
         <f t="shared" si="0"/>
         <v>2.3713737056616555</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="9">
         <f t="shared" si="1"/>
         <v>207</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="8">
         <v>-7.5</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="10">
         <f t="shared" si="2"/>
         <v>0.42169650342858223</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="9">
         <f t="shared" si="3"/>
         <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="11">
+      <c r="A18" s="8">
         <v>8</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="10">
         <f t="shared" si="0"/>
         <v>2.5118864315095806</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="9">
         <f t="shared" si="1"/>
         <v>208</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="8">
         <v>-8</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="10">
         <f t="shared" si="2"/>
         <v>0.3981071705534972</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="9">
         <f t="shared" si="3"/>
         <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="11">
+      <c r="A19" s="8">
         <v>8.5</v>
       </c>
-      <c r="B19" s="13">
+      <c r="B19" s="10">
         <f t="shared" si="0"/>
         <v>2.6607250597988097</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="9">
         <f t="shared" si="1"/>
         <v>209</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="8">
         <v>-8.5</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="10">
         <f t="shared" si="2"/>
         <v>0.37583740428844414</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="9">
         <f t="shared" si="3"/>
         <v>175</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="11">
+      <c r="A20" s="8">
         <v>9</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="10">
         <f t="shared" si="0"/>
         <v>2.8183829312644542</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="9">
         <f t="shared" si="1"/>
         <v>210</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="8">
         <v>-9</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="10">
         <f t="shared" si="2"/>
         <v>0.35481338923357542</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="9">
         <f t="shared" si="3"/>
         <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="11">
+      <c r="A21" s="8">
         <v>9.5</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B21" s="10">
         <f t="shared" si="0"/>
         <v>2.98538261891796</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="9">
         <f t="shared" si="1"/>
         <v>211</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="8">
         <v>-9.5</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="10">
         <f t="shared" si="2"/>
         <v>0.33496543915782762</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21" s="9">
         <f t="shared" si="3"/>
         <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="11">
+      <c r="A22" s="8">
         <v>10</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B22" s="10">
         <f t="shared" si="0"/>
         <v>3.1622776601683795</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="9">
         <f t="shared" si="1"/>
         <v>212</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="8">
         <v>-10</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="10">
         <f t="shared" si="2"/>
         <v>0.31622776601683794</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F22" s="9">
         <f t="shared" si="3"/>
         <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="11">
+      <c r="A23" s="8">
         <v>10.5</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B23" s="10">
         <f t="shared" si="0"/>
         <v>3.349654391578277</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="9">
         <f t="shared" si="1"/>
         <v>213</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="8">
         <v>-10.5</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="10">
         <f t="shared" si="2"/>
         <v>0.29853826189179594</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="9">
         <f t="shared" si="3"/>
         <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="11">
+      <c r="A24" s="8">
         <v>11</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B24" s="10">
         <f t="shared" si="0"/>
         <v>3.5481338923357555</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="9">
         <f t="shared" si="1"/>
         <v>214</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="8">
         <v>-11</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="10">
         <f t="shared" si="2"/>
         <v>0.28183829312644532</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="9">
         <f t="shared" si="3"/>
         <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="11">
+      <c r="A25" s="8">
         <v>11.5</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B25" s="10">
         <f t="shared" si="0"/>
         <v>3.7583740428844421</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="9">
         <f t="shared" si="1"/>
         <v>215</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="8">
         <v>-95.5</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="10">
         <f t="shared" si="2"/>
         <v>1.6788040181225564E-5</v>
       </c>
-      <c r="F25" s="12">
+      <c r="F25" s="9">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="11">
+      <c r="A26" s="8">
         <v>12</v>
       </c>
-      <c r="B26" s="13">
+      <c r="B26" s="10">
         <f t="shared" si="0"/>
         <v>3.9810717055349727</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="9">
         <f t="shared" si="1"/>
         <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="11">
+      <c r="A27" s="8">
         <v>12.5</v>
       </c>
-      <c r="B27" s="13">
+      <c r="B27" s="10">
         <f t="shared" si="0"/>
         <v>4.2169650342858231</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27" s="9">
         <f t="shared" si="1"/>
         <v>217</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="11">
+      <c r="A28" s="8">
         <v>13</v>
       </c>
-      <c r="B28" s="13">
+      <c r="B28" s="10">
         <f t="shared" si="0"/>
         <v>4.4668359215096318</v>
       </c>
-      <c r="C28" s="12">
+      <c r="C28" s="9">
         <f t="shared" si="1"/>
         <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="11">
+      <c r="A29" s="8">
         <v>13.5</v>
       </c>
-      <c r="B29" s="13">
+      <c r="B29" s="10">
         <f t="shared" si="0"/>
         <v>4.7315125896148054</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C29" s="9">
         <f t="shared" si="1"/>
         <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="11">
+      <c r="A30" s="8">
         <v>14</v>
       </c>
-      <c r="B30" s="13">
+      <c r="B30" s="10">
         <f t="shared" si="0"/>
         <v>5.0118723362727229</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30" s="9">
         <f t="shared" si="1"/>
         <v>220</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="11">
+      <c r="A31" s="8">
         <v>14.5</v>
       </c>
-      <c r="B31" s="13">
+      <c r="B31" s="10">
         <f t="shared" si="0"/>
         <v>5.3088444423098844</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="9">
         <f t="shared" si="1"/>
         <v>221</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="11">
+      <c r="A32" s="8">
         <v>15</v>
       </c>
-      <c r="B32" s="13">
+      <c r="B32" s="10">
         <f t="shared" si="0"/>
         <v>5.6234132519034921</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C32" s="9">
         <f t="shared" si="1"/>
         <v>222</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="11">
+      <c r="A33" s="8">
         <v>15.5</v>
       </c>
-      <c r="B33" s="13">
+      <c r="B33" s="10">
         <f t="shared" si="0"/>
         <v>5.9566214352901055</v>
       </c>
-      <c r="C33" s="12">
+      <c r="C33" s="9">
         <f t="shared" si="1"/>
         <v>223</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="11">
+      <c r="A34" s="8">
         <v>16</v>
       </c>
-      <c r="B34" s="13">
+      <c r="B34" s="10">
         <f t="shared" si="0"/>
         <v>6.3095734448019343</v>
       </c>
-      <c r="C34" s="12">
+      <c r="C34" s="9">
         <f t="shared" si="1"/>
         <v>224</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="11">
+      <c r="A35" s="8">
         <v>16.5</v>
       </c>
-      <c r="B35" s="13">
+      <c r="B35" s="10">
         <f t="shared" si="0"/>
         <v>6.6834391756861464</v>
       </c>
-      <c r="C35" s="12">
+      <c r="C35" s="9">
         <f t="shared" si="1"/>
         <v>225</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="11">
+      <c r="A36" s="8">
         <v>17</v>
       </c>
-      <c r="B36" s="13">
+      <c r="B36" s="10">
         <f t="shared" si="0"/>
         <v>7.0794578438413795</v>
       </c>
-      <c r="C36" s="12">
+      <c r="C36" s="9">
         <f t="shared" si="1"/>
         <v>226</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="11">
+      <c r="A37" s="8">
         <v>17.5</v>
       </c>
-      <c r="B37" s="13">
+      <c r="B37" s="10">
         <f t="shared" si="0"/>
         <v>7.4989420933245592</v>
       </c>
-      <c r="C37" s="12">
+      <c r="C37" s="9">
         <f t="shared" si="1"/>
         <v>227</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="11">
+      <c r="A38" s="8">
         <v>18</v>
       </c>
-      <c r="B38" s="13">
+      <c r="B38" s="10">
         <f t="shared" si="0"/>
         <v>7.9432823472428176</v>
       </c>
-      <c r="C38" s="12">
+      <c r="C38" s="9">
         <f t="shared" si="1"/>
         <v>228</v>
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="11">
+      <c r="A39" s="8">
         <v>18.5</v>
       </c>
-      <c r="B39" s="13">
+      <c r="B39" s="10">
         <f t="shared" si="0"/>
         <v>8.4139514164519547</v>
       </c>
-      <c r="C39" s="12">
+      <c r="C39" s="9">
         <f t="shared" si="1"/>
         <v>229</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="11">
+      <c r="A40" s="8">
         <v>19</v>
       </c>
-      <c r="B40" s="13">
+      <c r="B40" s="10">
         <f t="shared" si="0"/>
         <v>8.9125093813374576</v>
       </c>
-      <c r="C40" s="12">
+      <c r="C40" s="9">
         <f t="shared" si="1"/>
         <v>230</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="11">
+      <c r="A41" s="8">
         <v>19.5</v>
       </c>
-      <c r="B41" s="13">
+      <c r="B41" s="10">
         <f t="shared" si="0"/>
         <v>9.4406087628592346</v>
       </c>
-      <c r="C41" s="12">
+      <c r="C41" s="9">
         <f t="shared" si="1"/>
         <v>231</v>
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="11">
+      <c r="A42" s="8">
         <v>20</v>
       </c>
-      <c r="B42" s="13">
+      <c r="B42" s="10">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C42" s="12">
+      <c r="C42" s="9">
         <f t="shared" si="1"/>
         <v>232</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="11">
+      <c r="A43" s="8">
         <v>20.5</v>
       </c>
-      <c r="B43" s="13">
+      <c r="B43" s="10">
         <f t="shared" si="0"/>
         <v>10.592537251772889</v>
       </c>
-      <c r="C43" s="12">
+      <c r="C43" s="9">
         <f t="shared" si="1"/>
         <v>233</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="11">
+      <c r="A44" s="8">
         <v>21</v>
       </c>
-      <c r="B44" s="13">
+      <c r="B44" s="10">
         <f t="shared" si="0"/>
         <v>11.220184543019636</v>
       </c>
-      <c r="C44" s="12">
+      <c r="C44" s="9">
         <f t="shared" si="1"/>
         <v>234</v>
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="11">
+      <c r="A45" s="8">
         <v>21.5</v>
       </c>
-      <c r="B45" s="13">
+      <c r="B45" s="10">
         <f t="shared" si="0"/>
         <v>11.885022274370185</v>
       </c>
-      <c r="C45" s="12">
+      <c r="C45" s="9">
         <f t="shared" si="1"/>
         <v>235</v>
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="11">
+      <c r="A46" s="8">
         <v>22</v>
       </c>
-      <c r="B46" s="13">
+      <c r="B46" s="10">
         <f t="shared" si="0"/>
         <v>12.58925411794168</v>
       </c>
-      <c r="C46" s="12">
+      <c r="C46" s="9">
         <f t="shared" si="1"/>
         <v>236</v>
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="11">
+      <c r="A47" s="8">
         <v>22.5</v>
       </c>
-      <c r="B47" s="13">
+      <c r="B47" s="10">
         <f t="shared" si="0"/>
         <v>13.335214321633245</v>
       </c>
-      <c r="C47" s="12">
+      <c r="C47" s="9">
         <f t="shared" si="1"/>
         <v>237</v>
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="11">
+      <c r="A48" s="8">
         <v>23</v>
       </c>
-      <c r="B48" s="13">
+      <c r="B48" s="10">
         <f t="shared" si="0"/>
         <v>14.125375446227544</v>
       </c>
-      <c r="C48" s="12">
+      <c r="C48" s="9">
         <f t="shared" si="1"/>
         <v>238</v>
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="11">
+      <c r="A49" s="8">
         <v>23.5</v>
       </c>
-      <c r="B49" s="13">
+      <c r="B49" s="10">
         <f t="shared" si="0"/>
         <v>14.96235656094434</v>
       </c>
-      <c r="C49" s="12">
+      <c r="C49" s="9">
         <f t="shared" si="1"/>
         <v>239</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="11">
+      <c r="A50" s="8">
         <v>24</v>
       </c>
-      <c r="B50" s="13">
+      <c r="B50" s="10">
         <f t="shared" si="0"/>
         <v>15.848931924611136</v>
       </c>
-      <c r="C50" s="12">
+      <c r="C50" s="9">
         <f t="shared" si="1"/>
         <v>240</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="11">
+      <c r="A51" s="8">
         <v>24.5</v>
       </c>
-      <c r="B51" s="13">
+      <c r="B51" s="10">
         <f t="shared" si="0"/>
         <v>16.788040181225607</v>
       </c>
-      <c r="C51" s="12">
+      <c r="C51" s="9">
         <f t="shared" si="1"/>
         <v>241</v>
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="11">
+      <c r="A52" s="8">
         <v>25</v>
       </c>
-      <c r="B52" s="13">
+      <c r="B52" s="10">
         <f t="shared" si="0"/>
         <v>17.782794100389236</v>
       </c>
-      <c r="C52" s="12">
+      <c r="C52" s="9">
         <f t="shared" si="1"/>
         <v>242</v>
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="11">
+      <c r="A53" s="8">
         <v>25.5</v>
       </c>
-      <c r="B53" s="13">
+      <c r="B53" s="10">
         <f t="shared" si="0"/>
         <v>18.836490894898009</v>
       </c>
-      <c r="C53" s="12">
+      <c r="C53" s="9">
         <f t="shared" si="1"/>
         <v>243</v>
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="11">
+      <c r="A54" s="8">
         <v>26</v>
       </c>
-      <c r="B54" s="13">
+      <c r="B54" s="10">
         <f t="shared" si="0"/>
         <v>19.952623149688804</v>
       </c>
-      <c r="C54" s="12">
+      <c r="C54" s="9">
         <f t="shared" si="1"/>
         <v>244</v>
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="11">
+      <c r="A55" s="8">
         <v>26.5</v>
       </c>
-      <c r="B55" s="13">
+      <c r="B55" s="10">
         <f t="shared" si="0"/>
         <v>21.134890398366473</v>
       </c>
-      <c r="C55" s="12">
+      <c r="C55" s="9">
         <f t="shared" si="1"/>
         <v>245</v>
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="11">
+      <c r="A56" s="8">
         <v>27</v>
       </c>
-      <c r="B56" s="13">
+      <c r="B56" s="10">
         <f t="shared" si="0"/>
         <v>22.387211385683404</v>
       </c>
-      <c r="C56" s="12">
+      <c r="C56" s="9">
         <f t="shared" si="1"/>
         <v>246</v>
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="11">
+      <c r="A57" s="8">
         <v>27.5</v>
       </c>
-      <c r="B57" s="13">
+      <c r="B57" s="10">
         <f t="shared" si="0"/>
         <v>23.713737056616559</v>
       </c>
-      <c r="C57" s="12">
+      <c r="C57" s="9">
         <f t="shared" si="1"/>
         <v>247</v>
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="11">
+      <c r="A58" s="8">
         <v>28</v>
       </c>
-      <c r="B58" s="13">
+      <c r="B58" s="10">
         <f t="shared" si="0"/>
         <v>25.118864315095799</v>
       </c>
-      <c r="C58" s="12">
+      <c r="C58" s="9">
         <f t="shared" si="1"/>
         <v>248</v>
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="11">
+      <c r="A59" s="8">
         <v>28.5</v>
       </c>
-      <c r="B59" s="13">
+      <c r="B59" s="10">
         <f t="shared" si="0"/>
         <v>26.607250597988113</v>
       </c>
-      <c r="C59" s="12">
+      <c r="C59" s="9">
         <f t="shared" si="1"/>
         <v>249</v>
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="11">
+      <c r="A60" s="8">
         <v>29</v>
       </c>
-      <c r="B60" s="13">
+      <c r="B60" s="10">
         <f t="shared" si="0"/>
         <v>28.183829312644548</v>
       </c>
-      <c r="C60" s="12">
+      <c r="C60" s="9">
         <f t="shared" si="1"/>
         <v>250</v>
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="11">
+      <c r="A61" s="8">
         <v>29.5</v>
       </c>
-      <c r="B61" s="13">
+      <c r="B61" s="10">
         <f t="shared" si="0"/>
         <v>29.853826189179614</v>
       </c>
-      <c r="C61" s="12">
+      <c r="C61" s="9">
         <f t="shared" si="1"/>
         <v>251</v>
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="11">
+      <c r="A62" s="8">
         <v>30</v>
       </c>
-      <c r="B62" s="13">
+      <c r="B62" s="10">
         <f t="shared" si="0"/>
         <v>31.622776601683803</v>
       </c>
-      <c r="C62" s="12">
+      <c r="C62" s="9">
         <f t="shared" si="1"/>
         <v>252</v>
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="11">
+      <c r="A63" s="8">
         <v>30.5</v>
       </c>
-      <c r="B63" s="13">
+      <c r="B63" s="10">
         <f t="shared" si="0"/>
         <v>33.496543915782766</v>
       </c>
-      <c r="C63" s="12">
+      <c r="C63" s="9">
         <f t="shared" si="1"/>
         <v>253</v>
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="11">
+      <c r="A64" s="8">
         <v>31</v>
       </c>
-      <c r="B64" s="13">
+      <c r="B64" s="10">
         <f t="shared" si="0"/>
         <v>35.481338923357555</v>
       </c>
-      <c r="C64" s="12">
+      <c r="C64" s="9">
         <f t="shared" si="1"/>
         <v>254</v>
       </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="11">
+      <c r="A65" s="8">
         <v>31.5</v>
       </c>
-      <c r="B65" s="13">
+      <c r="B65" s="10">
         <f t="shared" si="0"/>
         <v>37.583740428844422</v>
       </c>
-      <c r="C65" s="12">
+      <c r="C65" s="9">
         <f t="shared" si="1"/>
         <v>255</v>
       </c>

</xml_diff>